<commit_message>
Update in the DNA table
Update in the DNA table of the samples located in /Namibia_project/Data/Nanodrop_measurements: I performed additional DNA cleaning because in our meeting we wanted to see if there are still contaminants in the samples that caused a division in the samples after the 16s gene sequencing (some samples showed a rapid plateau at 20 species, while others did not). Here in the table, I included Nanodrop and Quibit values before and after the extra cleaning. The cleaning improved the 260/230 ratio in several samples, but not the 260/280.
</commit_message>
<xml_diff>
--- a/Sequencing/analysis/16S_sequencing/tables/metadata.xlsx
+++ b/Sequencing/analysis/16S_sequencing/tables/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u_erazo/Documents/LABbook/2024/Namibia_sequencing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u_erazo/Documents/GitHub/Namibia_project/Sequencing/analysis/16S_sequencing/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{07875DD8-0418-C145-8785-010472B8CA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785DC37-45C5-7F41-AEBA-2BF0B7574312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{71E596EE-9B84-E249-AA04-9BD9BD2EBFE7}"/>
   </bookViews>
@@ -807,7 +807,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>